<commit_message>
Finalizing blue marlin models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7535581B-C537-8B49-BE1E-1A3BE8933DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF882C-5184-5246-9BB5-F42D8235441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>SWO</t>
+  </si>
+  <si>
+    <t>BLUM</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -664,6 +667,35 @@
         <v>0.2748852</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+      <c r="D6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E6">
+        <v>7400</v>
+      </c>
+      <c r="F6">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.84704000000000002</v>
+      </c>
+      <c r="H6">
+        <v>0.8458</v>
+      </c>
+      <c r="I6">
+        <v>0.57074950000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -671,10 +703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,6 +994,62 @@
         <v>4.9696959999999999</v>
       </c>
     </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>8.6223310000000009</v>
+      </c>
+      <c r="C6">
+        <v>3.2866019999999998</v>
+      </c>
+      <c r="D6">
+        <v>3.848922</v>
+      </c>
+      <c r="E6">
+        <v>11.864888000000001</v>
+      </c>
+      <c r="F6">
+        <v>6.7821210000000001</v>
+      </c>
+      <c r="G6">
+        <v>7.2555709999999998</v>
+      </c>
+      <c r="H6">
+        <v>5.8043889999999996</v>
+      </c>
+      <c r="I6">
+        <v>4.6561430000000001</v>
+      </c>
+      <c r="J6">
+        <v>9.3975980000000003</v>
+      </c>
+      <c r="K6">
+        <v>3.0482830000000001</v>
+      </c>
+      <c r="L6">
+        <v>3.0769760000000002</v>
+      </c>
+      <c r="M6">
+        <v>2.578935</v>
+      </c>
+      <c r="N6">
+        <v>7.5518299999999998</v>
+      </c>
+      <c r="O6">
+        <v>9.1212119999999999</v>
+      </c>
+      <c r="P6">
+        <v>2.528206</v>
+      </c>
+      <c r="Q6">
+        <v>6.522259</v>
+      </c>
+      <c r="R6">
+        <v>4.0537349999999996</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning frigate tuna models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF882C-5184-5246-9BB5-F42D8235441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77EBA82-D3F7-734C-BFFF-F1289F1FA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>BLUM</t>
+  </si>
+  <si>
+    <t>FRI</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,6 +699,35 @@
         <v>0.57074950000000002</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0.75</v>
+      </c>
+      <c r="D7">
+        <v>0.01</v>
+      </c>
+      <c r="E7">
+        <v>2850</v>
+      </c>
+      <c r="F7">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="G7">
+        <v>0.90271999999999997</v>
+      </c>
+      <c r="H7">
+        <v>0.90269999999999995</v>
+      </c>
+      <c r="I7">
+        <v>0.174483</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -703,10 +735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,6 +1082,62 @@
         <v>4.0537349999999996</v>
       </c>
     </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>3.3000340000000001</v>
+      </c>
+      <c r="C7">
+        <v>7.1003249999999998</v>
+      </c>
+      <c r="D7">
+        <v>1.3035350000000001</v>
+      </c>
+      <c r="E7">
+        <v>9.3021170000000009</v>
+      </c>
+      <c r="F7">
+        <v>10.819298</v>
+      </c>
+      <c r="G7">
+        <v>9.6629369999999994</v>
+      </c>
+      <c r="H7">
+        <v>1.159564</v>
+      </c>
+      <c r="I7">
+        <v>2.0677370000000002</v>
+      </c>
+      <c r="J7">
+        <v>3.1035659999999998</v>
+      </c>
+      <c r="K7">
+        <v>2.6029230000000001</v>
+      </c>
+      <c r="L7">
+        <v>5.7747339999999996</v>
+      </c>
+      <c r="M7">
+        <v>4.9527789999999996</v>
+      </c>
+      <c r="N7">
+        <v>8.9717479999999998</v>
+      </c>
+      <c r="O7">
+        <v>13.624162999999999</v>
+      </c>
+      <c r="P7">
+        <v>3.9452349999999998</v>
+      </c>
+      <c r="Q7">
+        <v>8.5025510000000004</v>
+      </c>
+      <c r="R7">
+        <v>3.8067540000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning bigeye tuna models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77EBA82-D3F7-734C-BFFF-F1289F1FA78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DCA929-E9F0-CA4D-A40D-F28266E9DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>FRI</t>
+  </si>
+  <si>
+    <t>BET</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,6 +731,35 @@
         <v>0.174483</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E8">
+        <v>6600</v>
+      </c>
+      <c r="F8">
+        <v>0.94620000000000004</v>
+      </c>
+      <c r="G8">
+        <v>0.86531999999999998</v>
+      </c>
+      <c r="H8">
+        <v>0.81940000000000002</v>
+      </c>
+      <c r="I8">
+        <v>0.2027264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -735,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,6 +1170,62 @@
         <v>3.8067540000000002</v>
       </c>
     </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>9.9593570000000007</v>
+      </c>
+      <c r="C8">
+        <v>3.2064059999999999</v>
+      </c>
+      <c r="D8">
+        <v>4.5297010000000002</v>
+      </c>
+      <c r="E8">
+        <v>3.1628660000000002</v>
+      </c>
+      <c r="F8">
+        <v>6.1421970000000004</v>
+      </c>
+      <c r="G8">
+        <v>10.81284</v>
+      </c>
+      <c r="H8">
+        <v>2.179942</v>
+      </c>
+      <c r="I8">
+        <v>4.6251899999999999</v>
+      </c>
+      <c r="J8">
+        <v>5.369122</v>
+      </c>
+      <c r="K8">
+        <v>2.399092</v>
+      </c>
+      <c r="L8">
+        <v>7.7990430000000002</v>
+      </c>
+      <c r="M8">
+        <v>1.399017</v>
+      </c>
+      <c r="N8">
+        <v>11.430529</v>
+      </c>
+      <c r="O8">
+        <v>10.927341999999999</v>
+      </c>
+      <c r="P8">
+        <v>6.3664379999999996</v>
+      </c>
+      <c r="Q8">
+        <v>6.462402</v>
+      </c>
+      <c r="R8">
+        <v>3.2285159999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning Pacific bluefin tuna models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DCA929-E9F0-CA4D-A40D-F28266E9DF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55D7326-5827-9C41-9E1A-FFA6984E085F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
+    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
   <sheets>
     <sheet name="optimal models" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>BET</t>
+  </si>
+  <si>
+    <t>BFT</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,6 +763,35 @@
         <v>0.2027264</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>0.01</v>
+      </c>
+      <c r="E9">
+        <v>3050</v>
+      </c>
+      <c r="F9">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="G9">
+        <v>0.99239999999999995</v>
+      </c>
+      <c r="H9">
+        <v>0.99080000000000001</v>
+      </c>
+      <c r="I9">
+        <v>2.8539740000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -767,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1226,6 +1258,62 @@
         <v>3.2285159999999999</v>
       </c>
     </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>1.2188098000000001</v>
+      </c>
+      <c r="C9">
+        <v>2.8458109</v>
+      </c>
+      <c r="D9">
+        <v>1.7593607</v>
+      </c>
+      <c r="E9">
+        <v>1.8752705000000001</v>
+      </c>
+      <c r="F9">
+        <v>2.6685229000000001</v>
+      </c>
+      <c r="G9">
+        <v>11.7668236</v>
+      </c>
+      <c r="H9">
+        <v>1.2960031999999999</v>
+      </c>
+      <c r="I9">
+        <v>1.5037383</v>
+      </c>
+      <c r="J9">
+        <v>0.4955521</v>
+      </c>
+      <c r="K9">
+        <v>6.1918363999999997</v>
+      </c>
+      <c r="L9">
+        <v>19.320694599999999</v>
+      </c>
+      <c r="M9">
+        <v>14.5793008</v>
+      </c>
+      <c r="N9">
+        <v>9.3146749999999994</v>
+      </c>
+      <c r="O9">
+        <v>16.998973899999999</v>
+      </c>
+      <c r="P9">
+        <v>1.3274022999999999</v>
+      </c>
+      <c r="Q9">
+        <v>4.2020749000000004</v>
+      </c>
+      <c r="R9">
+        <v>2.6351502</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning southern bluefin tuna models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB967F9F-E869-4E46-BCEF-61E98962B05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCCF29E-A3D5-4441-BDD7-C5C6AAA25C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>SAIL</t>
+  </si>
+  <si>
+    <t>SBFT</t>
   </si>
 </sst>
 </file>
@@ -524,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,6 +859,35 @@
         <v>0.12825739999999999</v>
       </c>
     </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0.75</v>
+      </c>
+      <c r="D12">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>2300</v>
+      </c>
+      <c r="F12">
+        <v>0.99780000000000002</v>
+      </c>
+      <c r="G12">
+        <v>0.98780000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="I12">
+        <v>2.8884E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -863,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1490,6 +1522,62 @@
         <v>9.0411579999999994</v>
       </c>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>9.7753189000000003</v>
+      </c>
+      <c r="C12">
+        <v>1.3711376</v>
+      </c>
+      <c r="D12">
+        <v>2.0247563</v>
+      </c>
+      <c r="E12">
+        <v>0.91375090000000003</v>
+      </c>
+      <c r="F12">
+        <v>0.97021469999999999</v>
+      </c>
+      <c r="G12">
+        <v>5.4405872999999998</v>
+      </c>
+      <c r="H12">
+        <v>7.3805990000000001</v>
+      </c>
+      <c r="I12">
+        <v>1.9768465</v>
+      </c>
+      <c r="J12">
+        <v>1.4763375000000001</v>
+      </c>
+      <c r="K12">
+        <v>0.16223000000000001</v>
+      </c>
+      <c r="L12">
+        <v>2.5284049</v>
+      </c>
+      <c r="M12">
+        <v>4.8537286999999996</v>
+      </c>
+      <c r="N12">
+        <v>42.1807406</v>
+      </c>
+      <c r="O12">
+        <v>13.918699999999999</v>
+      </c>
+      <c r="P12">
+        <v>0.26651190000000002</v>
+      </c>
+      <c r="Q12">
+        <v>4.7249812999999996</v>
+      </c>
+      <c r="R12">
+        <v>3.5153999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning slender tuna models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCCF29E-A3D5-4441-BDD7-C5C6AAA25C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FB511D-2DAF-F94E-BB89-873588D1DA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>SBFT</t>
+  </si>
+  <si>
+    <t>SLT</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -888,6 +891,35 @@
         <v>2.8884E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E13">
+        <v>1300</v>
+      </c>
+      <c r="F13">
+        <v>0.99709999999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.98146</v>
+      </c>
+      <c r="H13">
+        <v>0.98540000000000005</v>
+      </c>
+      <c r="I13">
+        <v>3.0286E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -895,10 +927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1578,6 +1610,62 @@
         <v>3.5153999999999998E-2</v>
       </c>
     </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>5.2984743999999999</v>
+      </c>
+      <c r="C13">
+        <v>17.114367000000001</v>
+      </c>
+      <c r="D13">
+        <v>7.4964237000000002</v>
+      </c>
+      <c r="E13">
+        <v>1.3195522</v>
+      </c>
+      <c r="F13">
+        <v>7.6811201999999996</v>
+      </c>
+      <c r="G13">
+        <v>6.6096602999999998</v>
+      </c>
+      <c r="H13">
+        <v>0.80767480000000003</v>
+      </c>
+      <c r="I13">
+        <v>0.67720720000000001</v>
+      </c>
+      <c r="J13">
+        <v>11.439719</v>
+      </c>
+      <c r="K13">
+        <v>2.8052522</v>
+      </c>
+      <c r="L13">
+        <v>6.9927041000000001</v>
+      </c>
+      <c r="M13">
+        <v>3.3238051</v>
+      </c>
+      <c r="N13">
+        <v>4.9016923999999999</v>
+      </c>
+      <c r="O13">
+        <v>18.894576099999998</v>
+      </c>
+      <c r="P13">
+        <v>1.3678341999999999</v>
+      </c>
+      <c r="Q13">
+        <v>2.2101546000000001</v>
+      </c>
+      <c r="R13">
+        <v>1.0597825000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning striped marlin models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E6A76-F1E5-D445-8374-4677690B1C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF4B4D4-21A6-9348-8F93-C9CAC27089A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
+    <workbookView xWindow="3680" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
   <sheets>
     <sheet name="optimal models" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>SHOS</t>
+  </si>
+  <si>
+    <t>STRM</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,6 +955,35 @@
         <v>0.30736580000000002</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E15">
+        <v>4000</v>
+      </c>
+      <c r="F15">
+        <v>0.93710000000000004</v>
+      </c>
+      <c r="G15">
+        <v>0.84406000000000003</v>
+      </c>
+      <c r="H15">
+        <v>0.85189999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.2006907</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -959,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1754,6 +1786,62 @@
         <v>1.2048220000000001</v>
       </c>
     </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>3.1714959999999999</v>
+      </c>
+      <c r="C15">
+        <v>7.7361649999999997</v>
+      </c>
+      <c r="D15">
+        <v>2.2644669999999998</v>
+      </c>
+      <c r="E15">
+        <v>4.1612609999999997</v>
+      </c>
+      <c r="F15">
+        <v>3.054748</v>
+      </c>
+      <c r="G15">
+        <v>10.896144</v>
+      </c>
+      <c r="H15">
+        <v>6.2197620000000002</v>
+      </c>
+      <c r="I15">
+        <v>6.9270160000000001</v>
+      </c>
+      <c r="J15">
+        <v>12.090750999999999</v>
+      </c>
+      <c r="K15">
+        <v>3.216059</v>
+      </c>
+      <c r="L15">
+        <v>10.520726</v>
+      </c>
+      <c r="M15">
+        <v>2.9078330000000001</v>
+      </c>
+      <c r="N15">
+        <v>3.3576030000000001</v>
+      </c>
+      <c r="O15">
+        <v>8.1469520000000006</v>
+      </c>
+      <c r="P15">
+        <v>2.077191</v>
+      </c>
+      <c r="Q15">
+        <v>9.2021270000000008</v>
+      </c>
+      <c r="R15">
+        <v>4.0497009999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rerunning longfin escolar models
</commit_message>
<xml_diff>
--- a/docs/BRT_model_outputs.xlsx
+++ b/docs/BRT_model_outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqkbuena/Documents/GitHub/LarvaDistModels/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF4B4D4-21A6-9348-8F93-C9CAC27089A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A89BD55-8642-6845-A38C-AB00D4F9D2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{C71D0CEA-5040-2740-95BA-74E660005632}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Taxon_Code</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>STRM</t>
+  </si>
+  <si>
+    <t>LESC</t>
   </si>
 </sst>
 </file>
@@ -536,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA7A54-CE70-BC44-88E9-3B8D5C5B6BE8}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,6 +987,35 @@
         <v>0.2006907</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.75</v>
+      </c>
+      <c r="D16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E16">
+        <v>6450</v>
+      </c>
+      <c r="F16">
+        <v>0.88570000000000004</v>
+      </c>
+      <c r="G16">
+        <v>0.80110000000000003</v>
+      </c>
+      <c r="H16">
+        <v>0.88470000000000004</v>
+      </c>
+      <c r="I16">
+        <v>0.127967</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -991,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65431BBD-853D-C44C-96AC-803D8FC2CBC6}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1842,6 +1874,62 @@
         <v>4.0497009999999998</v>
       </c>
     </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>3.2421185000000001</v>
+      </c>
+      <c r="C16">
+        <v>8.4286493999999994</v>
+      </c>
+      <c r="D16">
+        <v>1.5517163</v>
+      </c>
+      <c r="E16">
+        <v>2.3250592000000001</v>
+      </c>
+      <c r="F16">
+        <v>2.7232842000000002</v>
+      </c>
+      <c r="G16">
+        <v>6.7300705000000001</v>
+      </c>
+      <c r="H16">
+        <v>16.544630900000001</v>
+      </c>
+      <c r="I16">
+        <v>4.2541131999999999</v>
+      </c>
+      <c r="J16">
+        <v>6.3973209999999998</v>
+      </c>
+      <c r="K16">
+        <v>0.19126119999999999</v>
+      </c>
+      <c r="L16">
+        <v>1.4112623</v>
+      </c>
+      <c r="M16">
+        <v>6.3112580999999999</v>
+      </c>
+      <c r="N16">
+        <v>4.9988837999999998</v>
+      </c>
+      <c r="O16">
+        <v>4.9516112000000003</v>
+      </c>
+      <c r="P16">
+        <v>19.462621200000001</v>
+      </c>
+      <c r="Q16">
+        <v>9.1104018999999994</v>
+      </c>
+      <c r="R16">
+        <v>1.3657368999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>